<commit_message>
Summary of current results
</commit_message>
<xml_diff>
--- a/Result/summary.xlsx
+++ b/Result/summary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Micro - SF1</t>
   </si>
@@ -80,9 +80,6 @@
     <t>13.5|1.2</t>
   </si>
   <si>
-    <t>10.8|3.57</t>
-  </si>
-  <si>
     <t>272|80</t>
   </si>
   <si>
@@ -126,6 +123,72 @@
   </si>
   <si>
     <t>52.9|47.1</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>Times in Ms</t>
+  </si>
+  <si>
+    <t>9.6|3.57</t>
+  </si>
+  <si>
+    <t>8.5|0.54</t>
+  </si>
+  <si>
+    <t>116|2.3</t>
+  </si>
+  <si>
+    <t>111|35</t>
+  </si>
+  <si>
+    <t>TF GPU (Transfer|Exec)</t>
+  </si>
+  <si>
+    <t>TF TPU (Transfer|Exec)</t>
+  </si>
+  <si>
+    <t>7|0.2</t>
+  </si>
+  <si>
+    <t>78|2.7</t>
+  </si>
+  <si>
+    <t>22.3|0.06</t>
+  </si>
+  <si>
+    <t>79|0.5</t>
+  </si>
+  <si>
+    <t>79|649</t>
+  </si>
+  <si>
+    <t>19.2|0.12</t>
+  </si>
+  <si>
+    <t>86.6|1.1</t>
+  </si>
+  <si>
+    <t>0.05|0.06</t>
+  </si>
+  <si>
+    <t>0.06|0.08</t>
+  </si>
+  <si>
+    <t>22|50</t>
   </si>
 </sst>
 </file>
@@ -141,12 +204,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -161,8 +230,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,262 +515,488 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>460</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="2">
+        <v>470</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B9" s="1">
+        <v>380</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="1">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4900</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="1">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4560</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>143</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>518</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="1">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2">
+        <v>463</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6130</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="1">
+        <v>40</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>460</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B23" s="1">
+        <v>156</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="1">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>380</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>4900</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11">
-        <v>4560</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>143</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>518</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <v>6130</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>6</v>
-      </c>
-      <c r="B20">
-        <v>156</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>